<commit_message>
update completed system tests from all possible pairwise tests
</commit_message>
<xml_diff>
--- a/Team34/Tests34/system_test_with_2/system_test_with_pairwise_cases.xlsx
+++ b/Team34/Tests34/system_test_with_2/system_test_with_pairwise_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nauma\OneDrive\Desktop\NUS_MODULES\CS3203\spa_system_test_cases\Team34\Tests34\system_test_with_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865270DA-B6FA-4F38-B83B-0F287B46C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A98FA-71B5-4BC3-95F1-63AC81CE077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{E82867B0-7B47-4485-8A2B-ABCF81E6675B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
   <si>
     <t>Factors</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>stmt.stmt#</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -114,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,9 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +464,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -553,6 +563,9 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
@@ -561,6 +574,9 @@
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
@@ -569,6 +585,9 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
@@ -577,6 +596,9 @@
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
@@ -585,6 +607,9 @@
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
@@ -593,6 +618,9 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
@@ -618,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -626,7 +654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -634,7 +662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -642,15 +670,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -658,7 +689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -666,7 +697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -674,7 +705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -682,7 +713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -690,7 +721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -698,7 +729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -706,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -714,7 +745,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -722,7 +753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -730,7 +761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -738,15 +769,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C32" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -754,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -762,31 +796,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -794,7 +837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -802,7 +845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -810,7 +853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -818,7 +861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -826,7 +869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -834,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -842,7 +885,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -850,7 +893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>13</v>
       </c>

</xml_diff>